<commit_message>
Added gitignore and new executable
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="159" uniqueCount="70">
   <si>
     <t>Var1</t>
   </si>
@@ -124,6 +124,105 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -169,7 +268,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -234,90 +333,178 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>